<commit_message>
Clean up form formatting
</commit_message>
<xml_diff>
--- a/basic-forms/forms/app/android_app_launcher.xlsx
+++ b/basic-forms/forms/app/android_app_launcher.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId3"/>
@@ -291,7 +291,7 @@
     <t xml:space="preserve">android-app-launcher</t>
   </si>
   <si>
-    <t xml:space="preserve">string</t>
+    <t xml:space="preserve">text</t>
   </si>
   <si>
     <t xml:space="preserve">action</t>
@@ -351,7 +351,7 @@
     <t xml:space="preserve">coalesce(., “”)</t>
   </si>
   <si>
-    <t xml:space="preserve">true()</t>
+    <t xml:space="preserve">true</t>
   </si>
   <si>
     <t xml:space="preserve">form_title</t>
@@ -863,12 +863,12 @@
   </sheetPr>
   <dimension ref="A1:I1020"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C28" activeCellId="0" sqref="C28"/>
+      <selection pane="bottomRight" activeCell="G22" activeCellId="0" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10299,14 +10299,14 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="17.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="16.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="19.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="19.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="16.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="5" width="32.61"/>
   </cols>
@@ -10337,7 +10337,7 @@
       </c>
       <c r="C2" s="7" t="str">
         <f aca="true">TEXT(NOW(), "yyyymmddhhmmss")</f>
-        <v>20250213143751</v>
+        <v>20250213161449</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
Update with latest cht-conf changes again and remove NO_LABEL
</commit_message>
<xml_diff>
--- a/basic-forms/forms/app/android_app_launcher.xlsx
+++ b/basic-forms/forms/app/android_app_launcher.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
@@ -232,7 +232,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="48">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -285,19 +285,13 @@
     <t xml:space="preserve">camera_app</t>
   </si>
   <si>
-    <t xml:space="preserve">NO_LABEL</t>
-  </si>
-  <si>
     <t xml:space="preserve">android-app-launcher</t>
   </si>
   <si>
-    <t xml:space="preserve">text</t>
+    <t xml:space="preserve">hidden</t>
   </si>
   <si>
     <t xml:space="preserve">action</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hidden</t>
   </si>
   <si>
     <t xml:space="preserve">android.media.action.IMAGE_CAPTURE</t>
@@ -307,6 +301,9 @@
   </si>
   <si>
     <t xml:space="preserve">android-app-outputs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text</t>
   </si>
   <si>
     <t xml:space="preserve">data</t>
@@ -868,7 +865,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G22" activeCellId="0" sqref="G22"/>
+      <selection pane="bottomRight" activeCell="C27" activeCellId="0" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -963,32 +960,26 @@
       <c r="B5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>17</v>
-      </c>
+      <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F5" s="4"/>
       <c r="I5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="I6" s="4"/>
     </row>
@@ -997,43 +988,41 @@
         <v>12</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>17</v>
-      </c>
+      <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F7" s="4"/>
       <c r="I7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="F8" s="4"/>
       <c r="I8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -1043,7 +1032,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>16</v>
@@ -1056,7 +1045,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>13</v>
@@ -1081,10 +1070,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
@@ -1098,34 +1087,28 @@
         <v>12</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>17</v>
-      </c>
+      <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F14" s="4"/>
       <c r="I14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>17</v>
-      </c>
+      <c r="C15" s="4"/>
       <c r="D15" s="4"/>
-      <c r="E15" s="4" t="s">
-        <v>21</v>
-      </c>
+      <c r="E15" s="4"/>
       <c r="F15" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I15" s="4"/>
     </row>
@@ -1134,47 +1117,45 @@
         <v>12</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>17</v>
-      </c>
+      <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F16" s="4"/>
       <c r="I16" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="D17" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="I17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -1184,10 +1165,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -1197,10 +1178,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -10213,7 +10194,7 @@
       <c r="I1020" s="4"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A28:I10000 A27:B27 D27:I27 A2:I26">
+  <conditionalFormatting sqref="A28:I10000 A27:B27 D27:I27 A2:I26 C27">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>$A2="begin_group"</formula>
     </cfRule>
@@ -10235,9 +10216,9 @@
       <formula>AND(ISBLANK(B2), NOT(ISBLANK($A2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C28:C10000 C2:C26">
+  <conditionalFormatting sqref="C28:C10000 C2:C26 C27">
     <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>AND(ISBLANK(C2),NOT(OR(ISBLANK($A2),$A2="calculate")))</formula>
+      <formula>AND(ISBLANK(C2),NOT(OR(ISBLANK($A2),$A2="calculate",$A2="hidden")))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G10000">
@@ -10245,39 +10226,17 @@
       <formula>AND($A2="calculate", ISBLANK(G2))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C27">
-    <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>$A27="begin_group"</formula>
-    </cfRule>
-    <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>$A27="end_group"</formula>
-    </cfRule>
-    <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>$A27="begin_repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
-      <formula>$A27="end_repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>AND(ISBLANK($A27), NOT(ISBLANK(C27)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C27">
-    <cfRule type="expression" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>AND(ISBLANK(C27),NOT(OR(ISBLANK($A27),$A27="calculate")))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation allowBlank="true" error="If configuring a select, ensure your list name matches a list from the choices sheet." errorStyle="information" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="A1" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="If configuring a select, ensure your list name matches a list from the choices sheet." errorStyle="information" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1015" type="list">
-      <formula1>"begin_group,end_group,note,calculate,text,integer,decimal,select_one list_name,select_multiple list_name,date,time,datetime,begin_repeat,end_repeat,geopoint,geotrace,geoshape,start-geopoint,range,image,audio,video,file,rank,acknowledge,start,end,today"</formula1>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2:H1015" type="list">
+      <formula1>"true"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2:H1015" type="list">
-      <formula1>"true"</formula1>
+    <dataValidation allowBlank="true" error="If configuring a select, ensure your list name matches a list from the choices sheet." errorStyle="information" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1020" type="list">
+      <formula1>"begin_group,end_group,note,calculate,text,integer,decimal,select_one list_name,select_multiple list_name,date,time,datetime,begin_repeat,end_repeat,geopoint,geotrace,geoshape,start-geopoint,range,image,audio,video,file,rank,acknowledge,start,end,today,hid"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -10313,37 +10272,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="6" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="B2" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>46</v>
       </c>
       <c r="C2" s="7" t="str">
         <f aca="true">TEXT(NOW(), "yyyymmddhhmmss")</f>
-        <v>20250213161449</v>
+        <v>20251119131838</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove form_id from basic forms
</commit_message>
<xml_diff>
--- a/basic-forms/forms/app/android_app_launcher.xlsx
+++ b/basic-forms/forms/app/android_app_launcher.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId3"/>
@@ -184,9 +184,8 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">The unique ID that identifies this form to tools that use it. It may not contain spaces and must start with a letter or underscore. You should use a short, descriptive name and can use underscores to separate words. 
-For example: bench_inventory_2021
-You can change the form_title as much as you would like but if you change the form_id, it will be considered a different form definition.</t>
+          <t xml:space="preserve">The unique version code that identifies the current state of the form. A common convention is to use a format like yyyymmddrr. For example, 2017021501 is the 1st revision from Feb 15th, 2017.
+By default, this template uses a formula to create a date-based version that will update automatically.</t>
         </r>
       </text>
     </comment>
@@ -198,24 +197,11 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">The unique version code that identifies the current state of the form. A common convention is to use a format like yyyymmddrr. For example, 2017021501 is the 1st revision from Feb 15th, 2017.
-By default, this template uses a formula to create a date-based version that will update automatically.</t>
+          <t xml:space="preserve">Set to ‘pages’ to indicate that groups with the `field-list` appearance represent separate form pages (and all other questions will be shown on their own page). </t>
         </r>
       </text>
     </comment>
     <comment ref="D1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Set to ‘pages’ to indicate that groups with the `field-list` appearance represent separate form pages (and all other questions will be shown on their own page). </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -232,7 +218,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="46">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -354,9 +340,6 @@
     <t xml:space="preserve">form_title</t>
   </si>
   <si>
-    <t xml:space="preserve">form_id</t>
-  </si>
-  <si>
     <t xml:space="preserve">version</t>
   </si>
   <si>
@@ -367,9 +350,6 @@
   </si>
   <si>
     <t xml:space="preserve">Android App Launcher</t>
-  </si>
-  <si>
-    <t xml:space="preserve">android_app_launcher</t>
   </si>
   <si>
     <t xml:space="preserve">pages</t>
@@ -860,7 +840,7 @@
   </sheetPr>
   <dimension ref="A1:I1020"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
@@ -10194,7 +10174,7 @@
       <c r="I1020" s="4"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A28:I10000 A27:B27 D27:I27 A2:I26 C27">
+  <conditionalFormatting sqref="A2:I10000">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>$A2="begin_group"</formula>
     </cfRule>
@@ -10216,7 +10196,7 @@
       <formula>AND(ISBLANK(B2), NOT(ISBLANK($A2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C28:C10000 C2:C26 C27">
+  <conditionalFormatting sqref="C2:C10000">
     <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND(ISBLANK(C2),NOT(OR(ISBLANK($A2),$A2="calculate",$A2="hidden")))</formula>
     </cfRule>
@@ -10256,18 +10236,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="19.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="19.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="16.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="5" width="32.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="16.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="5" width="32.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10283,26 +10262,20 @@
       <c r="D1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="6" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="B2" s="7" t="str">
+        <f aca="true">TEXT(NOW(), "yyyymmddhhmmss")</f>
+        <v>20260114091903</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="C2" s="7" t="str">
-        <f aca="true">TEXT(NOW(), "yyyymmddhhmmss")</f>
-        <v>20251119131838</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: uplift to the new version of pyxform/cht-conf (#27)
</commit_message>
<xml_diff>
--- a/basic-forms/forms/app/android_app_launcher.xlsx
+++ b/basic-forms/forms/app/android_app_launcher.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId3"/>
@@ -184,9 +184,8 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">The unique ID that identifies this form to tools that use it. It may not contain spaces and must start with a letter or underscore. You should use a short, descriptive name and can use underscores to separate words. 
-For example: bench_inventory_2021
-You can change the form_title as much as you would like but if you change the form_id, it will be considered a different form definition.</t>
+          <t xml:space="preserve">The unique version code that identifies the current state of the form. A common convention is to use a format like yyyymmddrr. For example, 2017021501 is the 1st revision from Feb 15th, 2017.
+By default, this template uses a formula to create a date-based version that will update automatically.</t>
         </r>
       </text>
     </comment>
@@ -198,24 +197,11 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">The unique version code that identifies the current state of the form. A common convention is to use a format like yyyymmddrr. For example, 2017021501 is the 1st revision from Feb 15th, 2017.
-By default, this template uses a formula to create a date-based version that will update automatically.</t>
+          <t xml:space="preserve">Set to ‘pages’ to indicate that groups with the `field-list` appearance represent separate form pages (and all other questions will be shown on their own page). </t>
         </r>
       </text>
     </comment>
     <comment ref="D1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Set to ‘pages’ to indicate that groups with the `field-list` appearance represent separate form pages (and all other questions will be shown on their own page). </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -232,7 +218,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="46">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -285,19 +271,13 @@
     <t xml:space="preserve">camera_app</t>
   </si>
   <si>
-    <t xml:space="preserve">NO_LABEL</t>
-  </si>
-  <si>
     <t xml:space="preserve">android-app-launcher</t>
   </si>
   <si>
-    <t xml:space="preserve">text</t>
+    <t xml:space="preserve">hidden</t>
   </si>
   <si>
     <t xml:space="preserve">action</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hidden</t>
   </si>
   <si>
     <t xml:space="preserve">android.media.action.IMAGE_CAPTURE</t>
@@ -307,6 +287,9 @@
   </si>
   <si>
     <t xml:space="preserve">android-app-outputs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text</t>
   </si>
   <si>
     <t xml:space="preserve">data</t>
@@ -357,9 +340,6 @@
     <t xml:space="preserve">form_title</t>
   </si>
   <si>
-    <t xml:space="preserve">form_id</t>
-  </si>
-  <si>
     <t xml:space="preserve">version</t>
   </si>
   <si>
@@ -370,9 +350,6 @@
   </si>
   <si>
     <t xml:space="preserve">Android App Launcher</t>
-  </si>
-  <si>
-    <t xml:space="preserve">android_app_launcher</t>
   </si>
   <si>
     <t xml:space="preserve">pages</t>
@@ -863,12 +840,12 @@
   </sheetPr>
   <dimension ref="A1:I1020"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G22" activeCellId="0" sqref="G22"/>
+      <selection pane="bottomRight" activeCell="C27" activeCellId="0" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -963,32 +940,26 @@
       <c r="B5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>17</v>
-      </c>
+      <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F5" s="4"/>
       <c r="I5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="I6" s="4"/>
     </row>
@@ -997,43 +968,41 @@
         <v>12</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>17</v>
-      </c>
+      <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F7" s="4"/>
       <c r="I7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="F8" s="4"/>
       <c r="I8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -1043,7 +1012,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>16</v>
@@ -1056,7 +1025,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>13</v>
@@ -1081,10 +1050,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
@@ -1098,34 +1067,28 @@
         <v>12</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>17</v>
-      </c>
+      <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F14" s="4"/>
       <c r="I14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>17</v>
-      </c>
+      <c r="C15" s="4"/>
       <c r="D15" s="4"/>
-      <c r="E15" s="4" t="s">
-        <v>21</v>
-      </c>
+      <c r="E15" s="4"/>
       <c r="F15" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I15" s="4"/>
     </row>
@@ -1134,47 +1097,45 @@
         <v>12</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>17</v>
-      </c>
+      <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F16" s="4"/>
       <c r="I16" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="D17" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="I17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -1184,10 +1145,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -1197,10 +1158,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -10213,7 +10174,7 @@
       <c r="I1020" s="4"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A28:I10000 A27:B27 D27:I27 A2:I26">
+  <conditionalFormatting sqref="A2:I10000">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>$A2="begin_group"</formula>
     </cfRule>
@@ -10235,9 +10196,9 @@
       <formula>AND(ISBLANK(B2), NOT(ISBLANK($A2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C28:C10000 C2:C26">
+  <conditionalFormatting sqref="C2:C10000">
     <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>AND(ISBLANK(C2),NOT(OR(ISBLANK($A2),$A2="calculate")))</formula>
+      <formula>AND(ISBLANK(C2),NOT(OR(ISBLANK($A2),$A2="calculate",$A2="hidden")))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G10000">
@@ -10245,39 +10206,17 @@
       <formula>AND($A2="calculate", ISBLANK(G2))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C27">
-    <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>$A27="begin_group"</formula>
-    </cfRule>
-    <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>$A27="end_group"</formula>
-    </cfRule>
-    <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>$A27="begin_repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
-      <formula>$A27="end_repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>AND(ISBLANK($A27), NOT(ISBLANK(C27)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C27">
-    <cfRule type="expression" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>AND(ISBLANK(C27),NOT(OR(ISBLANK($A27),$A27="calculate")))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation allowBlank="true" error="If configuring a select, ensure your list name matches a list from the choices sheet." errorStyle="information" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="A1" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="If configuring a select, ensure your list name matches a list from the choices sheet." errorStyle="information" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1015" type="list">
-      <formula1>"begin_group,end_group,note,calculate,text,integer,decimal,select_one list_name,select_multiple list_name,date,time,datetime,begin_repeat,end_repeat,geopoint,geotrace,geoshape,start-geopoint,range,image,audio,video,file,rank,acknowledge,start,end,today"</formula1>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2:H1015" type="list">
+      <formula1>"true"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2:H1015" type="list">
-      <formula1>"true"</formula1>
+    <dataValidation allowBlank="true" error="If configuring a select, ensure your list name matches a list from the choices sheet." errorStyle="information" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1020" type="list">
+      <formula1>"begin_group,end_group,note,calculate,text,integer,decimal,select_one list_name,select_multiple list_name,date,time,datetime,begin_repeat,end_repeat,geopoint,geotrace,geoshape,start-geopoint,range,image,audio,video,file,rank,acknowledge,start,end,today,hid"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -10297,53 +10236,46 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="19.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="19.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="16.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="5" width="32.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="16.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="5" width="32.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="6" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="B2" s="7" t="str">
+        <f aca="true">TEXT(NOW(), "yyyymmddhhmmss")</f>
+        <v>20260114091903</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" s="7" t="str">
-        <f aca="true">TEXT(NOW(), "yyyymmddhhmmss")</f>
-        <v>20250213161449</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>